<commit_message>
add raw data from compute canada to git
</commit_message>
<xml_diff>
--- a/memory_raw_data.xlsx
+++ b/memory_raw_data.xlsx
@@ -1,33 +1,73 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DC0501-33E3-1D4F-87CD-02340239EC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-20320" yWindow="3580" windowWidth="20320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>sub(sub(sub(protectedDiv(cos(a1), a2), protectedDiv(protectedDiv(abs(a2), read(a0, a1)), abs(read(a0, cos(a1))))), write(a0, a1, write(a0, limit(limit(protectedDiv(cos(write(a0, 0, a1)), a2), protectedLog(a1), a1), protectedLog(a2), a1), a2))), protectedLog(0))</t>
+  </si>
+  <si>
+    <t>protectedDiv(sin(add(read(a0, a1), protectedDiv(a2, 0))), limit(a1, conditional(protectedDiv(write(a0, conditional(write(a0, 0, a1), a1), a2), a1), a2), a1))</t>
+  </si>
+  <si>
+    <t>sub(a2, add(sub(sub(sin(a2), read(a0, a2)), read(a0, a1)), protectedDiv(cos(protectedDiv(read(a0, 0), a2)), write(a0, a1, a2))))</t>
+  </si>
+  <si>
+    <t>protectedDiv(limit(sin(0), conditional(protectedDiv(sin(a2), protectedDiv(a2, a1)), read(a0, 0)), sub(conditional(0, limit(0, limit(a2, 0, a2), read(a0, 0))), abs(add(protectedDiv(cos(add(a1, protectedLog(a2))), conditional(a1, a1)), write(a0, 0, a1))))), sin(a2))</t>
+  </si>
+  <si>
+    <t>sub(protectedLog(protectedDiv(protectedLog(protectedDiv(a1, conditional(read(a0, read(a0, a1)), a2))), sub(a1, a2))), protectedDiv(conditional(read(a0, 0), write(a0, limit(add(0, write(a0, a2, cos(a2))), 0, 0), a1)), a2))</t>
+  </si>
+  <si>
+    <t>sub(add(add(write(a0, 0, limit(read(a0, conditional(0, a1)), a1, add(a2, a1))), read(a0, read(a0, a1))), read(a0, protectedDiv(abs(0), conditional(cos(abs(a1)), protectedDiv(a2, 0))))), sub(protectedLog(cos(0)), a1))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, sin(0)), add(add(protectedDiv(a2, abs(read(a0, abs(protectedDiv(a2, a2))))), add(write(a0, read(a0, 0), a2), protectedDiv(a2, protectedDiv(a2, read(a0, protectedLog(0)))))), a2))</t>
+  </si>
+  <si>
+    <t>sub(sub(read(a0, sin(conditional(0, sin(a1)))), read(a0, write(a0, protectedLog(conditional(sub(a1, 0), 0)), write(a0, a2, protectedDiv(protectedLog(abs(protectedLog(cos(protectedLog(abs(a1)))))), a2))))), protectedDiv(a1, a2))</t>
+  </si>
+  <si>
+    <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
+  </si>
+  <si>
+    <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +86,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -407,161 +388,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="12.5" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Row 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ads</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sub(sub(sub(protectedDiv(cos(a1), a2), protectedDiv(protectedDiv(abs(a2), read(a0, a1)), abs(read(a0, cos(a1))))), write(a0, a1, write(a0, limit(limit(protectedDiv(cos(write(a0, 0, a1)), a2), protectedLog(a1), a1), protectedLog(a2), a1), a2))), protectedLog(0))</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>-236</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>protectedDiv(sin(add(read(a0, a1), protectedDiv(a2, 0))), limit(a1, conditional(protectedDiv(write(a0, conditional(write(a0, 0, a1), a1), a2), a1), a2), a1))</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>-977</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sub(a2, add(sub(sub(sin(a2), read(a0, a2)), read(a0, a1)), protectedDiv(cos(protectedDiv(read(a0, 0), a2)), write(a0, a1, a2))))</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>-193</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>protectedDiv(limit(sin(0), conditional(protectedDiv(sin(a2), protectedDiv(a2, a1)), read(a0, 0)), sub(conditional(0, limit(0, limit(a2, 0, a2), read(a0, 0))), abs(add(protectedDiv(cos(add(a1, protectedLog(a2))), conditional(a1, a1)), write(a0, 0, a1))))), sin(a2))</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>-134</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sub(protectedLog(protectedDiv(protectedLog(protectedDiv(a1, conditional(read(a0, read(a0, a1)), a2))), sub(a1, a2))), protectedDiv(conditional(read(a0, 0), write(a0, limit(add(0, write(a0, a2, cos(a2))), 0, 0), a1)), a2))</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>-224</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>sub(add(add(write(a0, 0, limit(read(a0, conditional(0, a1)), a1, add(a2, a1))), read(a0, read(a0, a1))), read(a0, protectedDiv(abs(0), conditional(cos(abs(a1)), protectedDiv(a2, 0))))), sub(protectedLog(cos(0)), a1))</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>-938</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>sub(read(a0, sin(0)), add(add(protectedDiv(a2, abs(read(a0, abs(protectedDiv(a2, a2))))), add(write(a0, read(a0, 0), a2), protectedDiv(a2, protectedDiv(a2, read(a0, protectedLog(0)))))), a2))</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>-477</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>sub(sub(read(a0, sin(conditional(0, sin(a1)))), read(a0, write(a0, protectedLog(conditional(sub(a1, 0), 0)), write(a0, a2, protectedDiv(protectedLog(abs(protectedLog(cos(protectedLog(abs(a1)))))), a2))))), protectedDiv(a1, a2))</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>-116</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>protectedDiv(sub(a2, read(a0, read(a0, a1))), protectedLog(conditional(protectedDiv(a1, cos(a2)), limit(protectedDiv(sin(sub(a2, a2)), protectedLog(limit(a1, protectedDiv(a1, a2), a2))), a1, protectedLog(write(a0, read(a0, cos(conditional(a2, read(a0, a1)))), write(a0, sin(a1), sin(sin(a2)))))))))</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>-117</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>sub(write(a0, 0, protectedDiv(read(a0, a1), cos(limit(write(a0, cos(abs(limit(a1, abs(abs(0)), 0))), a1), sub(a2, 0), a1)))), write(a0, add(abs(cos(add(a1, a1))), sub(add(sub(sin(sub(0, a1)), 0), 0), a1)), limit(0, protectedDiv(limit(read(a0, read(a0, a2)), read(a0, sub(a2, a2)), sub(0, sub(abs(write(a0, a1, conditional(protectedDiv(a1, protectedLog(cos(a2))), a2))), a2))), a2), protectedDiv(read(a0, add(a2, a2)), protectedLog(cos(a2))))))</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>-114</v>
       </c>
     </row>

</xml_diff>